<commit_message>
Do statistics for copy counting and process areas.
</commit_message>
<xml_diff>
--- a/metrics/fluid_metrics.xlsx
+++ b/metrics/fluid_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD4\research\dflowmap\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6754095-EE79-4D9A-A0E0-8BFBD23AF2DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FE6C23-CCF6-49C0-AED8-178A60DEBD40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1680,16 +1680,16 @@
         <v>58</v>
       </c>
       <c r="B51" s="8">
-        <v>2487.9102720000001</v>
+        <v>2625.0014253999998</v>
       </c>
       <c r="C51" s="8">
-        <v>29151.684053787998</v>
+        <v>24847.628011699937</v>
       </c>
       <c r="D51" s="8">
-        <v>4115</v>
+        <v>3384</v>
       </c>
       <c r="E51" s="8">
-        <v>8463.8192000000017</v>
+        <v>8678.7405399999989</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2456,16 +2456,16 @@
         <v>5</v>
       </c>
       <c r="B95" s="8">
-        <v>2527.1538221999999</v>
+        <v>3058.1267253999999</v>
       </c>
       <c r="C95" s="8">
-        <v>33443.759826933798</v>
+        <v>28986.304910366598</v>
       </c>
       <c r="D95" s="8">
-        <v>4572</v>
+        <v>3384</v>
       </c>
       <c r="E95" s="8">
-        <v>8467.6862199999996</v>
+        <v>9268.3685399999995</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2617,16 +2617,16 @@
         <v>56</v>
       </c>
       <c r="B104" s="8">
-        <v>181.579634</v>
+        <v>324.12076519999999</v>
       </c>
       <c r="C104" s="8">
-        <v>709.04627165266675</v>
+        <v>988.09399305185264</v>
       </c>
       <c r="D104" s="8">
-        <v>785</v>
+        <v>577</v>
       </c>
       <c r="E104" s="8">
-        <v>506.52940000000001</v>
+        <v>768.72852</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
update the way dflowmap generates metrics for Function Unit.
And avoid including/calling external optimizer if LOGIC_OPTIMIZER is set to be false.
</commit_message>
<xml_diff>
--- a/metrics/fluid_metrics.xlsx
+++ b/metrics/fluid_metrics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD4\research\dflowmap\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3783C3-649B-44F4-AF0B-7DB086E8FD93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B8388A-BF34-4ACB-9228-B23BB91BAB53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>Leak Power (nW)</t>
   </si>
@@ -496,6 +496,24 @@
   </si>
   <si>
     <t>0eqc2047_0eqc2047_r1eqc0_1eqc0_c1addr3_c0queryr4_0eqc2047_r6eqc0_1eqc0_c1addr8_c0queryr9_0eqc2047_r11eqc0_1eqc0_c1addr13_c0queryr14_0eqc2047_r16eqc0_2eqc0_c0addr18_r19queryc2_0eqc2047_r21eqc0_1eqc0_c1addr23_c0queryr24_32_32_64_1_2_2_2_2_2_1_1_1_1_2_2_1_1_1_2_2_1_1_1_2_2_1_1_1_2_2_1_1_1_2_2_</t>
+  </si>
+  <si>
+    <t>latch1</t>
+  </si>
+  <si>
+    <t>latch8</t>
+  </si>
+  <si>
+    <t>latch16</t>
+  </si>
+  <si>
+    <t>latch32</t>
+  </si>
+  <si>
+    <t>latch64</t>
+  </si>
+  <si>
+    <t>twoToOne</t>
   </si>
 </sst>
 </file>
@@ -590,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -636,6 +654,9 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A148" sqref="A148"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3578,6 +3599,114 @@
         <v>485.81916000000001</v>
       </c>
     </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B153" s="3"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
+      <c r="E153" s="3"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B154" s="19">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="C154" s="12">
+        <v>6099.5</v>
+      </c>
+      <c r="D154" s="12">
+        <v>95</v>
+      </c>
+      <c r="E154" s="19">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B155" s="19">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="C155" s="12">
+        <v>7.4192499999999999</v>
+      </c>
+      <c r="D155" s="12">
+        <v>59</v>
+      </c>
+      <c r="E155" s="19">
+        <v>2.117</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B156" s="19">
+        <v>4.3879999999999999</v>
+      </c>
+      <c r="C156" s="12">
+        <v>64.071698999999995</v>
+      </c>
+      <c r="D156" s="12">
+        <v>59</v>
+      </c>
+      <c r="E156" s="19">
+        <v>16.934999999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B157" s="19">
+        <v>8.7159999999999993</v>
+      </c>
+      <c r="C157" s="12">
+        <v>126.26843700000001</v>
+      </c>
+      <c r="D157" s="12">
+        <v>59</v>
+      </c>
+      <c r="E157" s="19">
+        <v>33.869999999999997</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B158" s="19">
+        <v>17.460999999999999</v>
+      </c>
+      <c r="C158" s="12">
+        <v>250.16790599999999</v>
+      </c>
+      <c r="D158" s="12">
+        <v>59</v>
+      </c>
+      <c r="E158" s="19">
+        <v>67.739999999999995</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B159" s="19">
+        <v>35.029000000000003</v>
+      </c>
+      <c r="C159" s="12">
+        <v>544.45188199999996</v>
+      </c>
+      <c r="D159" s="12">
+        <v>59</v>
+      </c>
+      <c r="E159" s="19">
+        <v>135.48099999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Backup for doing logic optimizations for nested ACT expressions.
</commit_message>
<xml_diff>
--- a/metrics/fluid_metrics.xlsx
+++ b/metrics/fluid_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD4\research\dflowmap\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B8388A-BF34-4ACB-9228-B23BB91BAB53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10599C81-88BA-4936-ABB2-E9E7BD66D274}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28704" yWindow="-96" windowWidth="28992" windowHeight="15792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3613,7 +3613,7 @@
         <v>0.63600000000000001</v>
       </c>
       <c r="C154" s="12">
-        <v>6099.5</v>
+        <v>6.1</v>
       </c>
       <c r="D154" s="12">
         <v>95</v>

</xml_diff>